<commit_message>
[what] Update the analyze.xlsx
</commit_message>
<xml_diff>
--- a/data/analyze.xlsx
+++ b/data/analyze.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\git\filter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E111D59B-AF38-44B6-A7E2-551854D73B0F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E962838E-2C6A-4A7E-ABD1-1F476C0E7581}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9495"/>
   </bookViews>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>search time (per 1000 time)</t>
-  </si>
   <si>
     <t>欄1</t>
   </si>
@@ -68,6 +65,10 @@
   </si>
   <si>
     <t>信賴度(95.0%)</t>
+  </si>
+  <si>
+    <t>search time (A total of 1000 rounds were run, and the keywords were filtered 1000 times per a round.)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1051,14 +1052,14 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1066,7 +1067,7 @@
         <v>153</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -1082,7 +1083,7 @@
         <v>92</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>98.911000000000001</v>
@@ -1093,7 +1094,7 @@
         <v>94</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
         <v>0.38233919791496945</v>
@@ -1104,7 +1105,7 @@
         <v>93</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1">
         <v>96</v>
@@ -1115,7 +1116,7 @@
         <v>98</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1">
         <v>92</v>
@@ -1126,7 +1127,7 @@
         <v>98</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1">
         <v>12.090627041732045</v>
@@ -1137,7 +1138,7 @@
         <v>101</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1">
         <v>146.18326226226216</v>
@@ -1148,7 +1149,7 @@
         <v>129</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1">
         <v>48.176082220954143</v>
@@ -1159,7 +1160,7 @@
         <v>104</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1">
         <v>5.5766387584483468</v>
@@ -1170,7 +1171,7 @@
         <v>90</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="1">
         <v>162</v>
@@ -1181,7 +1182,7 @@
         <v>101</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="1">
         <v>89</v>
@@ -1192,7 +1193,7 @@
         <v>91</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" s="1">
         <v>251</v>
@@ -1203,7 +1204,7 @@
         <v>93</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" s="1">
         <v>98911</v>
@@ -1214,7 +1215,7 @@
         <v>92</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16" s="1">
         <v>1000</v>
@@ -1225,7 +1226,7 @@
         <v>96</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="2">
         <v>0.75028006028505734</v>

</xml_diff>